<commit_message>
Database first try to build
</commit_message>
<xml_diff>
--- a/Extract.xlsx
+++ b/Extract.xlsx
@@ -22,7 +22,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Sign-in Count</t>
+    <t>Sign-in-Count</t>
   </si>
   <si>
     <t>James Smith</t>
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>

<commit_message>
Uer control to update data
</commit_message>
<xml_diff>
--- a/Extract.xlsx
+++ b/Extract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\64384\PycharmProjects\ELEC498\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6134C8-0DD7-4A9D-A32F-88CA09B76F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B50E270-4EC8-43CA-86A9-F19B6D0D6A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Sign-in-Count</t>
+  </si>
+  <si>
+    <t>Total-Count</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -257,13 +260,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -570,15 +587,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,8 +608,11 @@
       <c r="D1" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -602,8 +622,11 @@
       <c r="C2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -614,7 +637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -625,7 +648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -636,7 +659,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -647,7 +670,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -658,7 +681,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -669,7 +692,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -680,7 +703,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -691,7 +714,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -702,7 +725,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -713,7 +736,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -724,7 +747,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -735,7 +758,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -746,7 +769,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>